<commit_message>
Testdaten wurden erweitert mit barID und angepassten HappyHourZeiten
</commit_message>
<xml_diff>
--- a/documents/marketing/Daten - Happy Hour.xlsx
+++ b/documents/marketing/Daten - Happy Hour.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="94">
   <si>
     <t>barID</t>
   </si>
@@ -235,9 +235,6 @@
     <t>0711 27397933</t>
   </si>
   <si>
-    <t>Bar du Frisco</t>
-  </si>
-  <si>
     <t>0711 8886163</t>
   </si>
   <si>
@@ -260,6 +257,45 @@
   </si>
   <si>
     <t>Alle Cocktails und Longdrinks 1,50€ günstiger</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>5001a910e4b0d8ae05eec43f</t>
+  </si>
+  <si>
+    <t>4c9513a258d4b60c93e12e29</t>
+  </si>
+  <si>
+    <t>4c87654b47cc224b99a4b09f</t>
+  </si>
+  <si>
+    <t>4b7ee121f964a520590630e3</t>
+  </si>
+  <si>
+    <t>4e0e11c27d8bb178a8a53262</t>
+  </si>
+  <si>
+    <t>4bd89025f645c9b6ab47a8e0</t>
+  </si>
+  <si>
+    <t>4b771002f964a52062792ee3</t>
+  </si>
+  <si>
+    <t>4c2a4e48355cef3b27facc56</t>
+  </si>
+  <si>
+    <t>4fe4bdd5e4b0d43f1fceec16</t>
+  </si>
+  <si>
+    <t>Bar di Frisco</t>
+  </si>
+  <si>
+    <t>4e6f30be52b1706317b5b8f6</t>
+  </si>
+  <si>
+    <t>4b7d9923f964a520f4c82fe3</t>
   </si>
 </sst>
 </file>
@@ -304,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -313,7 +349,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -621,9 +656,9 @@
   <dimension ref="A1:M577"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A41"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,6 +933,9 @@
       <c r="E8" s="5">
         <v>0.70833333333333337</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G8" t="s">
         <v>20</v>
       </c>
@@ -965,6 +1003,9 @@
       <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
       <c r="D10" t="s">
         <v>39</v>
       </c>
@@ -1003,6 +1044,9 @@
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
       <c r="D11" t="s">
         <v>40</v>
       </c>
@@ -1035,6 +1079,9 @@
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
       <c r="D12" t="s">
         <v>40</v>
       </c>
@@ -1058,6 +1105,9 @@
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
       <c r="D13" t="s">
         <v>45</v>
       </c>
@@ -1078,6 +1128,9 @@
       <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
       <c r="D14" t="s">
         <v>44</v>
       </c>
@@ -1104,11 +1157,17 @@
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
       <c r="D15" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="5">
         <v>0.45833333333333331</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1133,11 +1192,17 @@
       <c r="B16" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
       <c r="D16" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="5">
         <v>0.5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="L16" t="s">
         <v>20</v>
@@ -1153,11 +1218,17 @@
       <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
       <c r="D17" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="5">
         <v>0.70833333333333337</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
@@ -1170,6 +1241,9 @@
       <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
       <c r="D18" t="s">
         <v>28</v>
       </c>
@@ -1205,6 +1279,9 @@
       <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
       <c r="D19" t="s">
         <v>55</v>
       </c>
@@ -1243,6 +1320,9 @@
       <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
@@ -1275,6 +1355,9 @@
       <c r="B21" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
       <c r="D21" t="s">
         <v>56</v>
       </c>
@@ -1298,6 +1381,9 @@
       <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
       <c r="D22" t="s">
         <v>57</v>
       </c>
@@ -1327,6 +1413,9 @@
       <c r="B23" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
       <c r="D23" t="s">
         <v>57</v>
       </c>
@@ -1350,6 +1439,9 @@
       <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
       <c r="D24" t="s">
         <v>57</v>
       </c>
@@ -1370,6 +1462,9 @@
       <c r="B25" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
       <c r="D25" t="s">
         <v>60</v>
       </c>
@@ -1402,6 +1497,9 @@
       <c r="B26" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
       <c r="D26" t="s">
         <v>63</v>
       </c>
@@ -1434,6 +1532,9 @@
       <c r="B27" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
       <c r="D27" t="s">
         <v>63</v>
       </c>
@@ -1454,6 +1555,9 @@
       <c r="B28" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
       <c r="D28" t="s">
         <v>63</v>
       </c>
@@ -1474,6 +1578,9 @@
       <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
       <c r="D29" t="s">
         <v>50</v>
       </c>
@@ -1512,6 +1619,9 @@
       <c r="B30" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
       <c r="D30" t="s">
         <v>66</v>
       </c>
@@ -1532,6 +1642,9 @@
       <c r="B31" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
       <c r="D31" t="s">
         <v>50</v>
       </c>
@@ -1552,6 +1665,9 @@
       <c r="B32" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
       <c r="D32" t="s">
         <v>67</v>
       </c>
@@ -1572,6 +1688,9 @@
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
       <c r="D33" t="s">
         <v>68</v>
       </c>
@@ -1592,6 +1711,9 @@
       <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
       <c r="D34" t="s">
         <v>69</v>
       </c>
@@ -1615,6 +1737,9 @@
       <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
       <c r="D35" t="s">
         <v>70</v>
       </c>
@@ -1635,6 +1760,9 @@
       <c r="B36" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
       <c r="D36" t="s">
         <v>50</v>
       </c>
@@ -1650,13 +1778,16 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" t="s">
         <v>74</v>
-      </c>
-      <c r="D37" t="s">
-        <v>75</v>
       </c>
       <c r="E37" s="5">
         <v>0.75</v>
@@ -1688,19 +1819,22 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>74</v>
+      <c r="C38" t="s">
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="5">
         <v>0.75</v>
       </c>
-      <c r="F38" s="6">
-        <v>1</v>
+      <c r="F38" s="5">
+        <v>0</v>
       </c>
       <c r="I38" t="s">
         <v>20</v>
@@ -1708,13 +1842,16 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" t="s">
         <v>78</v>
-      </c>
-      <c r="D39" t="s">
-        <v>79</v>
       </c>
       <c r="E39" s="5">
         <v>0.95833333333333337</v>
@@ -1728,13 +1865,16 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>78</v>
+      <c r="C40" t="s">
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E40" s="5">
         <v>0.95833333333333337</v>
@@ -1748,13 +1888,16 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>78</v>
+      <c r="C41" t="s">
+        <v>93</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="5">
         <v>0.95833333333333337</v>

</xml_diff>